<commit_message>
ended simulation early (too many values). restarted with few parameter combinations.
</commit_message>
<xml_diff>
--- a/SUMMARY/simulation_summary_06-24-2014.xlsx
+++ b/SUMMARY/simulation_summary_06-24-2014.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="77">
   <si>
     <t>Functions used:</t>
   </si>
@@ -232,22 +232,19 @@
     <t>Simulation ended:</t>
   </si>
   <si>
-    <t>0, 0.2, 0.4, 0.6</t>
-  </si>
-  <si>
     <t>1:99, 50:50, 99:1, 99:99</t>
   </si>
   <si>
-    <t>06-24-2014 - FP&amp;SAV - WIND() - const NtoP - light_limitation - Scheffer vers</t>
-  </si>
-  <si>
     <t>0.1, 1, 2, 3,… 10</t>
   </si>
   <si>
-    <t>all, up</t>
-  </si>
-  <si>
-    <t>6/24/2014 ~7:00AM</t>
+    <t>all</t>
+  </si>
+  <si>
+    <t>06-24-2014 - FP&amp;SAV - light_WIND() - const NtoP - light_limitation - Scheffer vers</t>
+  </si>
+  <si>
+    <t>6/24/2014 ~12:30PM</t>
   </si>
 </sst>
 </file>
@@ -344,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -375,6 +372,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -680,7 +680,7 @@
   <dimension ref="A1:L43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -702,7 +702,7 @@
         <v>70</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>37</v>
@@ -1073,7 +1073,7 @@
         <v>4</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>41</v>
@@ -1177,7 +1177,7 @@
         <v>11</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>48</v>
@@ -1200,10 +1200,10 @@
         <v>50</v>
       </c>
       <c r="B27" s="4">
-        <v>4</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>72</v>
+        <v>1</v>
+      </c>
+      <c r="C27" s="19">
+        <v>0.2</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>49</v>
@@ -1226,10 +1226,10 @@
         <v>51</v>
       </c>
       <c r="B28" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J28" s="4">
         <v>0.02</v>
@@ -1267,7 +1267,7 @@
       </c>
       <c r="B30" s="3">
         <f>B22*B23*B24*B25*B26*B27*B28*B29</f>
-        <v>9504</v>
+        <v>1188</v>
       </c>
       <c r="J30" s="4">
         <v>0.02</v>
@@ -1306,7 +1306,7 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>

</xml_diff>